<commit_message>
UPDATE NEO FEEDER SUPPORT
UPDATE NEO FEEDER SUPPORT
</commit_message>
<xml_diff>
--- a/upload/sample/kelas_sample_baru.xlsx
+++ b/upload/sample/kelas_sample_baru.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\feeder\upload\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\feeder-importer\upload\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D70C68-5111-451B-8E7A-BB299954EF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20391" windowHeight="8368"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,13 +22,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
     <author>wildantea</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="1" shapeId="0">
+    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -154,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -185,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0">
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -224,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="1" shapeId="0">
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -263,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="1" shapeId="0">
+    <comment ref="G1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -299,6 +300,59 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Info : Boleh Kosong
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{FB2EDB7B-2B38-42B6-9FA3-CECDDF7387AF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lingkup Kelas</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1 : Internal
+2 : External
+3 : Campuran</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{D56B1769-89DB-4D07-AF45-88EB7F3D7723}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mode Kuliah
+O : Online
+F : Offline
+M : Campuran</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -308,7 +362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>semester</t>
   </si>
@@ -331,27 +385,36 @@
     <t>Tanggal Akhir Efektir</t>
   </si>
   <si>
-    <t>KDA0009</t>
-  </si>
-  <si>
-    <t>Bahasa Indonesia</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>Tentang Bahasa Indonesia</t>
+    <t>Lingkup</t>
+  </si>
+  <si>
+    <t>Mode Kuliah</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	IF15702</t>
+  </si>
+  <si>
+    <t>Sistem Multimedia</t>
+  </si>
+  <si>
+    <t>Tentang Sistem Multimedia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="166" formatCode="00"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
@@ -369,6 +432,29 @@
       <sz val="9"/>
       <name val="SimSun"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -426,7 +512,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -439,17 +525,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,25 +847,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.65" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.75" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
+    <col min="3" max="3" width="30.375" customWidth="1"/>
+    <col min="4" max="4" width="14.125" customWidth="1"/>
+    <col min="5" max="5" width="23.75" customWidth="1"/>
+    <col min="6" max="6" width="17.75" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="8.625" customWidth="1"/>
+    <col min="9" max="9" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,83 +889,92 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>20151</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>20211</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="6">
+        <v>44228</v>
+      </c>
+      <c r="G2" s="6">
+        <v>44237</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7">
-        <v>42401</v>
-      </c>
-      <c r="G2" s="7">
-        <v>42410</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F16" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="7"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="7"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="7"/>
+      <c r="F19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.50902777777777797" footer="0.50902777777777797"/>
@@ -877,24 +983,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.65" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.50902777777777797" footer="0.50902777777777797"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.65" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.50902777777777797" footer="0.50902777777777797"/>
 </worksheet>

</xml_diff>